<commit_message>
DDL e DML concluídos
</commit_message>
<xml_diff>
--- a/modelagem/físico/HROADS-físico.xlsx
+++ b/modelagem/físico/HROADS-físico.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24401"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CCA61D8-6098-495C-BCFE-A7A2F0DD599E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45BAFEFA-1413-40BF-BEC4-2FA31B6F7C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>tipoHabilidade</t>
   </si>
@@ -76,10 +76,31 @@
     <t>classe</t>
   </si>
   <si>
+    <t>nomeClasse</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Bárbaro</t>
+  </si>
+  <si>
+    <t>Cruzado</t>
+  </si>
+  <si>
+    <t>Caçadora de Demônios</t>
+  </si>
+  <si>
+    <t>Monge</t>
+  </si>
+  <si>
+    <t>Necromante</t>
+  </si>
+  <si>
     <t>personagem</t>
   </si>
   <si>
-    <t>nomeClasse</t>
+    <t>Feiticeiro</t>
   </si>
   <si>
     <t>idPersonagem</t>
@@ -88,50 +109,47 @@
     <t>nomePersonagem</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Bárbaro</t>
+    <t>vidaMax</t>
+  </si>
+  <si>
+    <t>manaMax</t>
+  </si>
+  <si>
+    <t>dataCriacao</t>
+  </si>
+  <si>
+    <t>dataAtualizacao</t>
+  </si>
+  <si>
+    <t>Arcanista</t>
   </si>
   <si>
     <t>DeuBug</t>
   </si>
   <si>
-    <t>Cruzado</t>
-  </si>
-  <si>
     <t>BitBug</t>
   </si>
   <si>
-    <t>Caçadora de Demônios</t>
-  </si>
-  <si>
     <t>Fer8</t>
-  </si>
-  <si>
-    <t>Monge</t>
-  </si>
-  <si>
-    <t>Necromante</t>
-  </si>
-  <si>
-    <t>Feiticeiro</t>
-  </si>
-  <si>
-    <t>Arcanista</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,11 +182,13 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -488,7 +508,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H2" sqref="H2:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -500,8 +520,7 @@
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -521,25 +540,25 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -547,7 +566,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1">
@@ -573,7 +592,7 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1">
@@ -599,7 +618,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1">
@@ -625,7 +644,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="2"/>
@@ -639,7 +658,7 @@
     <row r="7" spans="1:16">
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="5"/>
       <c r="H7" s="1">
         <v>4</v>
       </c>
@@ -651,9 +670,6 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
       <c r="H8" s="1">
         <v>4</v>
       </c>
@@ -665,24 +681,15 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="H9" s="1">
         <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -690,19 +697,10 @@
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="H10" s="1">
         <v>6</v>
       </c>
@@ -715,24 +713,15 @@
       <c r="A11" s="1">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
-        <v>23</v>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>4</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H11" s="1">
         <v>7</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J11" s="1"/>
     </row>
@@ -740,80 +729,151 @@
       <c r="A12" s="1">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="7"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="F13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="7"/>
+      <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="F14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="7"/>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="F15" s="1"/>
+      <c r="J15" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="7"/>
+      <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="1">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="1">
+        <v>100</v>
+      </c>
+      <c r="H16" s="1">
+        <v>80</v>
+      </c>
+      <c r="I16" s="6">
+        <v>43483</v>
+      </c>
+      <c r="J16" s="6">
+        <v>44418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="1">
+        <v>70</v>
+      </c>
+      <c r="H17" s="1">
+        <v>100</v>
+      </c>
+      <c r="I17" s="6">
+        <v>42446</v>
+      </c>
+      <c r="J17" s="7">
+        <v>44418</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1"/>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="1">
+        <v>75</v>
+      </c>
+      <c r="H18" s="1">
+        <v>60</v>
+      </c>
+      <c r="I18" s="6">
+        <v>43177</v>
+      </c>
+      <c r="J18" s="7">
+        <v>44418</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>